<commit_message>
Discuss about game engine
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Web Development\monopoly\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam Đỗ\My Code\monopoly\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF35DAC-B29B-4905-A4A2-9E964D28FB67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{F568A7F5-FB83-4B91-A1B6-E3F448F2DA71}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,8 +17,9 @@
     <sheet name="Component" sheetId="4" r:id="rId3"/>
     <sheet name="Component's state" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
+    <sheet name="Công việc cần làm" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
   <si>
     <t>Ô</t>
   </si>
@@ -286,20 +286,134 @@
     <t>Player has location</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>componentDidMount()</t>
   </si>
   <si>
     <t>Use grid for location</t>
+  </si>
+  <si>
+    <t>Công việc</t>
+  </si>
+  <si>
+    <t>Người làm</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Di chuyển </t>
+  </si>
+  <si>
+    <t>Để sau</t>
+  </si>
+  <si>
+    <t>state()</t>
+  </si>
+  <si>
+    <t>Trong 1 turn, player 1 onRoll() ---&gt; truyền cho player move(5)---&gt; hiện game messages --&gt; thao tác --&gt; gọi funcition đổi lượt (thay đổi isTurn người chơi khác thành true)</t>
+  </si>
+  <si>
+    <t>Thao tác ô đặc biệt --&gt; Gọi chức năng ô đặc biệt --&gt; render lại player</t>
+  </si>
+  <si>
+    <t>Thao tác ô đất --&gt; Check sở hữu -&gt;&gt; false: thao tác mua, true: xây thêm nhà hoặc mất tiền</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store </t>
+  </si>
+  <si>
+    <t>PlayerInf</t>
+  </si>
+  <si>
+    <t>currntPlayer</t>
+  </si>
+  <si>
+    <t>currentMoney</t>
+  </si>
+  <si>
+    <t>playerArr[]</t>
+  </si>
+  <si>
+    <t>moneyArr[]</t>
+  </si>
+  <si>
+    <t>posID</t>
+  </si>
+  <si>
+    <t>posRow</t>
+  </si>
+  <si>
+    <t>posCol</t>
+  </si>
+  <si>
+    <t>Hoàn thiện bàn cờ, thiết kế luôn 4 quân cờ trong 1 ô</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>ô máy bay: name</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>messageType: thông báo hoặc thao tác</t>
+  </si>
+  <si>
+    <t>messageContent: "content từ special, "bạn đã mất ${Ơ} tiền"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tùy thuộc vào type gọi hàm tương ứng: </t>
+  </si>
+  <si>
+    <t>SlotInf</t>
+  </si>
+  <si>
+    <t>slotName</t>
+  </si>
+  <si>
+    <t>oneHousePrice</t>
+  </si>
+  <si>
+    <t>twoHousePrice</t>
+  </si>
+  <si>
+    <t>threeHouse</t>
+  </si>
+  <si>
+    <t>……</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>HistoryInf</t>
+  </si>
+  <si>
+    <t>Viết function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiết kế dữ liệu game </t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Chuyển dữ liệu thành mảng object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên hàm và tham số truyền vào </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,8 +456,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +489,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -378,10 +504,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -395,8 +522,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,7 +837,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318AD7AD-FE71-4AB2-9F7E-204FD3D5952E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1788,7 +1917,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37186B19-81C9-407C-9CB1-33A4A2E23997}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1859,11 +1988,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9568406-B1BC-49B2-B058-1023E040590D}">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1873,82 +2002,85 @@
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>74</v>
       </c>
@@ -1965,75 +2097,160 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C18BB8-B344-422B-B476-7BF4262777B7}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>66</v>
       </c>
+      <c r="B1" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="C1" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
       <c r="C2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1843A670-5DC2-4BBB-8481-DCC7407870B9}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2053,10 +2270,100 @@
         <v>82</v>
       </c>
       <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>